<commit_message>
validado prova modulo 3 pos ead adm e finanças
</commit_message>
<xml_diff>
--- a/PosEAD  Adm e Finanças/Modulo 3/Provas/Gabarito das Provas.xlsx
+++ b/PosEAD  Adm e Finanças/Modulo 3/Provas/Gabarito das Provas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cezar Nakase\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cezar\projetos\PosEAD  Adm e Finanças\Modulo 3\Provas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
   <si>
     <t>Prova Gestão Estratégica de Custos</t>
   </si>
@@ -34,12 +34,27 @@
   <si>
     <t>Prova Gestão Integrada de Riscos</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Conferido</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +78,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -78,7 +101,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -101,23 +124,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,190 +435,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="4">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4">
-        <v>5</v>
-      </c>
-      <c r="F3" s="4">
-        <v>6</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3">
         <v>7</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>8</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>9</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="4">
-        <v>3</v>
-      </c>
-      <c r="D9" s="4">
-        <v>4</v>
-      </c>
-      <c r="E9" s="4">
-        <v>5</v>
-      </c>
-      <c r="F9" s="4">
-        <v>6</v>
-      </c>
-      <c r="G9" s="4">
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>6</v>
+      </c>
+      <c r="G9" s="3">
         <v>7</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>8</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>9</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="15" spans="1:10" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="15" spans="1:12" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>1</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="C15" s="4">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4">
-        <v>4</v>
-      </c>
-      <c r="E15" s="4">
-        <v>5</v>
-      </c>
-      <c r="F15" s="4">
-        <v>6</v>
-      </c>
-      <c r="G15" s="4">
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3">
+        <v>5</v>
+      </c>
+      <c r="F15" s="3">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3">
         <v>7</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>8</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>9</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>